<commit_message>
New major update 2.0
Big changes in the program :
- Model now generate a table of entities instead of ints
- Model now generate the table from the database datas
- GameWindow now integrate a KeyListener system
- Some comportements and movements possibilities added in the controller
- Useless classes and interfaces were removed
- The different packages can now properly communicate between themselves
- The launch of the program is now done properly from the main

Others :
- Javadoc has been updated
- The JXR report has been updated
- Added a new JUnit test (not functionnal yet)
</commit_message>
<xml_diff>
--- a/Consignes et documents initiaux/Grille dévaluation.xlsx
+++ b/Consignes et documents initiaux/Grille dévaluation.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Scolaire\Exia.CESI\Projets\06 - Boulder Dash\Boulder_Dash\Consignes et documents initiaux\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="13908" windowHeight="8376"/>
   </bookViews>
@@ -10,7 +15,7 @@
     <sheet name="Projet" sheetId="1" r:id="rId1"/>
     <sheet name="Cahier de test" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -20,7 +25,7 @@
     <author>Diet Jean-Aymeric</author>
   </authors>
   <commentList>
-    <comment ref="B4" authorId="0">
+    <comment ref="B4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -34,7 +39,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0">
+    <comment ref="C4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -330,7 +335,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -996,6 +1001,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1043,7 +1051,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1076,9 +1084,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1111,6 +1136,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1290,7 +1332,7 @@
   <dimension ref="A1:X21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:W1"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1345,42 +1387,42 @@
       <c r="S1" s="39"/>
       <c r="T1" s="36" t="str">
         <f>IF(X1&gt;=(C3*I3*O3*U3)*0.7,"A",IF(AD1&gt;=(C3*I3*O3*U3)*0.5,"B",IF(AD1&gt;=(C3*I3*O3*U3)*0.3,"C","D")))</f>
-        <v>D</v>
+        <v>A</v>
       </c>
       <c r="U1" s="36"/>
       <c r="V1" s="36"/>
       <c r="W1" s="37"/>
       <c r="X1">
         <f>B3*H3*N3*T3</f>
-        <v>0</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:24" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="13">
         <f>IF(B4="A",4,IF(B4="B",3,IF(B4="C",1,0)))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C3" s="13">
         <v>4</v>
       </c>
       <c r="H3" s="13">
         <f>IF(H4="A",4,IF(H4="B",3,IF(H4="C",1,0)))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I3" s="3">
         <v>4</v>
       </c>
       <c r="N3" s="13">
         <f>IF(N4="A",4,IF(N4="B",3,IF(N4="C",1,0)))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O3" s="13">
         <v>4</v>
       </c>
       <c r="T3" s="13">
         <f>IF(T4="A",4,IF(T4="B",3,IF(T4="C",1,0)))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U3" s="13">
         <v>1</v>
@@ -1392,14 +1434,14 @@
       </c>
       <c r="B4" s="12" t="str">
         <f>IF(D4&gt;SUM(C5:C19)*0.7,"A",IF(D4&gt;=SUM(C5:C19)*0.5,"B",IF(D4&gt;=SUM(C5:C19)*0.3,"C","D")))</f>
-        <v>D</v>
+        <v>B</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="12">
         <f>SUM(D5:D21)</f>
-        <v>0</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>3</v>
@@ -1409,14 +1451,14 @@
       </c>
       <c r="H4" s="21" t="str">
         <f>IF(J4&gt;SUM(I5:I21)*0.7,"A",IF(J4&gt;=SUM(I5:I21)*0.5,"B",IF(J4&gt;=SUM(I5:I21)*0.3,"C","D")))</f>
-        <v>D</v>
+        <v>A</v>
       </c>
       <c r="I4" s="21" t="s">
         <v>12</v>
       </c>
       <c r="J4" s="29">
         <f>SUM(J5:J21)</f>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="K4" s="21" t="s">
         <v>3</v>
@@ -1426,14 +1468,14 @@
       </c>
       <c r="N4" s="21" t="str">
         <f>IF(P4&gt;SUM(O5:O13)*0.7,"A",IF(P4&gt;=SUM(O5:O13)*0.5,"B",IF(P4&gt;=SUM(O5:O13)*0.3,"C","D")))</f>
-        <v>D</v>
+        <v>A</v>
       </c>
       <c r="O4" s="21" t="s">
         <v>12</v>
       </c>
       <c r="P4" s="21">
         <f>SUM(P5:P14)</f>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="Q4" s="29" t="s">
         <v>3</v>
@@ -1443,14 +1485,14 @@
       </c>
       <c r="T4" s="21" t="str">
         <f>IF(PRODUCT(V5:V14),"A","D")</f>
-        <v>D</v>
+        <v>A</v>
       </c>
       <c r="U4" s="21" t="s">
         <v>12</v>
       </c>
       <c r="V4" s="21">
         <f>PRODUCT(V5:V14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W4" s="29" t="s">
         <v>3</v>
@@ -1460,13 +1502,15 @@
       <c r="A5" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="16"/>
+      <c r="B5" s="16">
+        <v>1</v>
+      </c>
       <c r="C5" s="5">
         <v>2</v>
       </c>
       <c r="D5" s="5">
         <f>(B5/E5)*C5</f>
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="E5" s="5">
         <v>5</v>
@@ -1474,13 +1518,15 @@
       <c r="G5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="19"/>
+      <c r="H5" s="19">
+        <v>2</v>
+      </c>
       <c r="I5" s="14">
         <v>3</v>
       </c>
       <c r="J5" s="30">
         <f>(H5/K5)*I5</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K5" s="22">
         <v>2</v>
@@ -1488,13 +1534,15 @@
       <c r="M5" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="N5" s="19"/>
+      <c r="N5" s="19">
+        <v>2</v>
+      </c>
       <c r="O5" s="14">
         <v>3</v>
       </c>
       <c r="P5" s="14">
         <f>(N5/Q5)*O5</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q5" s="33">
         <v>2</v>
@@ -1502,13 +1550,15 @@
       <c r="S5" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="T5" s="19"/>
+      <c r="T5" s="19">
+        <v>1</v>
+      </c>
       <c r="U5" s="14">
         <v>1</v>
       </c>
       <c r="V5" s="14">
         <f>(T5/W5)*U5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W5" s="33">
         <v>1</v>
@@ -1532,13 +1582,15 @@
       <c r="G6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="17"/>
+      <c r="H6" s="17">
+        <v>1</v>
+      </c>
       <c r="I6" s="6">
         <v>3</v>
       </c>
       <c r="J6" s="31">
         <f t="shared" ref="J6:J19" si="1">(H6/K6)*I6</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K6" s="23">
         <v>1</v>
@@ -1546,13 +1598,15 @@
       <c r="M6" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="N6" s="17"/>
+      <c r="N6" s="17">
+        <v>1</v>
+      </c>
       <c r="O6" s="6">
         <v>3</v>
       </c>
       <c r="P6" s="6">
         <f t="shared" ref="P6:P12" si="2">(N6/Q6)*O6</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q6" s="34">
         <v>1</v>
@@ -1560,13 +1614,15 @@
       <c r="S6" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="T6" s="17"/>
+      <c r="T6" s="17">
+        <v>1</v>
+      </c>
       <c r="U6" s="6">
         <v>1</v>
       </c>
       <c r="V6" s="6">
         <f t="shared" ref="V6:V14" si="3">(T6/W6)*U6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W6" s="34">
         <v>1</v>
@@ -1576,13 +1632,15 @@
       <c r="A7" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="17"/>
+      <c r="B7" s="17">
+        <v>1</v>
+      </c>
       <c r="C7" s="6">
         <v>3</v>
       </c>
       <c r="D7" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E7" s="6">
         <v>1</v>
@@ -1590,13 +1648,15 @@
       <c r="G7" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="17"/>
+      <c r="H7" s="17">
+        <v>2</v>
+      </c>
       <c r="I7" s="6">
         <v>2</v>
       </c>
       <c r="J7" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K7" s="23">
         <v>2</v>
@@ -1604,13 +1664,15 @@
       <c r="M7" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="N7" s="17"/>
+      <c r="N7" s="17">
+        <v>1</v>
+      </c>
       <c r="O7" s="6">
         <v>2</v>
       </c>
       <c r="P7" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q7" s="34">
         <v>1</v>
@@ -1618,13 +1680,15 @@
       <c r="S7" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="T7" s="17"/>
+      <c r="T7" s="17">
+        <v>1</v>
+      </c>
       <c r="U7" s="6">
         <v>1</v>
       </c>
       <c r="V7" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W7" s="34">
         <v>1</v>
@@ -1634,13 +1698,15 @@
       <c r="A8" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="17"/>
+      <c r="B8" s="17">
+        <v>1</v>
+      </c>
       <c r="C8" s="6">
         <v>3</v>
       </c>
       <c r="D8" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E8" s="6">
         <v>1</v>
@@ -1648,13 +1714,15 @@
       <c r="G8" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="17"/>
+      <c r="H8" s="17">
+        <v>2</v>
+      </c>
       <c r="I8" s="6">
         <v>3</v>
       </c>
       <c r="J8" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K8" s="23">
         <v>2</v>
@@ -1662,13 +1730,15 @@
       <c r="M8" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="17"/>
+      <c r="N8" s="17">
+        <v>1</v>
+      </c>
       <c r="O8" s="6">
         <v>2</v>
       </c>
       <c r="P8" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q8" s="34">
         <v>1</v>
@@ -1676,13 +1746,15 @@
       <c r="S8" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="T8" s="17"/>
+      <c r="T8" s="17">
+        <v>1</v>
+      </c>
       <c r="U8" s="6">
         <v>1</v>
       </c>
       <c r="V8" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W8" s="34">
         <v>1</v>
@@ -1706,13 +1778,15 @@
       <c r="G9" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="17"/>
+      <c r="H9" s="17">
+        <v>2</v>
+      </c>
       <c r="I9" s="6">
         <v>2</v>
       </c>
       <c r="J9" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K9" s="23">
         <v>2</v>
@@ -1720,13 +1794,15 @@
       <c r="M9" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="N9" s="17"/>
+      <c r="N9" s="17">
+        <v>2</v>
+      </c>
       <c r="O9" s="6">
         <v>2</v>
       </c>
       <c r="P9" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q9" s="34">
         <v>2</v>
@@ -1734,13 +1810,15 @@
       <c r="S9" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="T9" s="17"/>
+      <c r="T9" s="17">
+        <v>1</v>
+      </c>
       <c r="U9" s="6">
         <v>1</v>
       </c>
       <c r="V9" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W9" s="34">
         <v>1</v>
@@ -1750,13 +1828,15 @@
       <c r="A10" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="17"/>
+      <c r="B10" s="17">
+        <v>1</v>
+      </c>
       <c r="C10" s="6">
         <v>3</v>
       </c>
       <c r="D10" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E10" s="6">
         <v>1</v>
@@ -1764,13 +1844,15 @@
       <c r="G10" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="17"/>
+      <c r="H10" s="17">
+        <v>1</v>
+      </c>
       <c r="I10" s="6">
         <v>3</v>
       </c>
       <c r="J10" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K10" s="23">
         <v>1</v>
@@ -1778,13 +1860,15 @@
       <c r="M10" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="N10" s="17"/>
+      <c r="N10" s="17">
+        <v>2</v>
+      </c>
       <c r="O10" s="6">
         <v>2</v>
       </c>
       <c r="P10" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q10" s="34">
         <v>2</v>
@@ -1792,13 +1876,15 @@
       <c r="S10" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="T10" s="17"/>
+      <c r="T10" s="17">
+        <v>1</v>
+      </c>
       <c r="U10" s="6">
         <v>1</v>
       </c>
       <c r="V10" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W10" s="34">
         <v>1</v>
@@ -1822,13 +1908,15 @@
       <c r="G11" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="17"/>
+      <c r="H11" s="17">
+        <v>1</v>
+      </c>
       <c r="I11" s="6">
         <v>3</v>
       </c>
       <c r="J11" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K11" s="23">
         <v>1</v>
@@ -1836,13 +1924,15 @@
       <c r="M11" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="N11" s="17"/>
+      <c r="N11" s="17">
+        <v>2</v>
+      </c>
       <c r="O11" s="6">
         <v>2</v>
       </c>
       <c r="P11" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q11" s="34">
         <v>2</v>
@@ -1850,13 +1940,15 @@
       <c r="S11" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="T11" s="17"/>
+      <c r="T11" s="17">
+        <v>1</v>
+      </c>
       <c r="U11" s="6">
         <v>1</v>
       </c>
       <c r="V11" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W11" s="34">
         <v>1</v>
@@ -1880,13 +1972,15 @@
       <c r="G12" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="17"/>
+      <c r="H12" s="17">
+        <v>1</v>
+      </c>
       <c r="I12" s="6">
         <v>3</v>
       </c>
       <c r="J12" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K12" s="23">
         <v>1</v>
@@ -1894,13 +1988,15 @@
       <c r="M12" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="N12" s="17"/>
+      <c r="N12" s="17">
+        <v>1</v>
+      </c>
       <c r="O12" s="6">
         <v>2</v>
       </c>
       <c r="P12" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q12" s="34">
         <v>1</v>
@@ -1908,13 +2004,15 @@
       <c r="S12" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="T12" s="17"/>
+      <c r="T12" s="17">
+        <v>1</v>
+      </c>
       <c r="U12" s="6">
         <v>1</v>
       </c>
       <c r="V12" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W12" s="34">
         <v>1</v>
@@ -1938,13 +2036,15 @@
       <c r="G13" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="H13" s="17"/>
+      <c r="H13" s="17">
+        <v>1</v>
+      </c>
       <c r="I13" s="6">
         <v>3</v>
       </c>
       <c r="J13" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K13" s="23">
         <v>1</v>
@@ -1952,13 +2052,15 @@
       <c r="M13" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="N13" s="17"/>
+      <c r="N13" s="17">
+        <v>2</v>
+      </c>
       <c r="O13" s="6">
         <v>2</v>
       </c>
       <c r="P13" s="6">
         <f t="shared" ref="P13" si="4">(N13/Q13)*O13</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q13" s="34">
         <v>2</v>
@@ -1966,13 +2068,15 @@
       <c r="S13" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="T13" s="17"/>
+      <c r="T13" s="17">
+        <v>1</v>
+      </c>
       <c r="U13" s="6">
         <v>1</v>
       </c>
       <c r="V13" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W13" s="34">
         <v>1</v>
@@ -1982,13 +2086,15 @@
       <c r="A14" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="17"/>
+      <c r="B14" s="17">
+        <v>1</v>
+      </c>
       <c r="C14" s="6">
         <v>3</v>
       </c>
       <c r="D14" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E14" s="6">
         <v>1</v>
@@ -1996,13 +2102,15 @@
       <c r="G14" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="17"/>
+      <c r="H14" s="17">
+        <v>2</v>
+      </c>
       <c r="I14" s="6">
         <v>2</v>
       </c>
       <c r="J14" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K14" s="23">
         <v>2</v>
@@ -2010,13 +2118,15 @@
       <c r="M14" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="N14" s="18"/>
+      <c r="N14" s="18">
+        <v>3</v>
+      </c>
       <c r="O14" s="7">
         <v>3</v>
       </c>
       <c r="P14" s="7">
         <f t="shared" ref="P14" si="5">(N14/Q14)*O14</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q14" s="35">
         <v>3</v>
@@ -2024,13 +2134,15 @@
       <c r="S14" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="T14" s="18"/>
+      <c r="T14" s="18">
+        <v>1</v>
+      </c>
       <c r="U14" s="7">
         <v>1</v>
       </c>
       <c r="V14" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W14" s="35">
         <v>1</v>
@@ -2040,13 +2152,15 @@
       <c r="A15" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="17"/>
+      <c r="B15" s="17">
+        <v>1</v>
+      </c>
       <c r="C15" s="6">
         <v>2</v>
       </c>
       <c r="D15" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E15" s="6">
         <v>1</v>
@@ -2054,13 +2168,15 @@
       <c r="G15" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="17"/>
+      <c r="H15" s="17">
+        <v>2</v>
+      </c>
       <c r="I15" s="6">
         <v>2</v>
       </c>
       <c r="J15" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K15" s="23">
         <v>2</v>
@@ -2070,13 +2186,15 @@
       <c r="A16" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="17"/>
+      <c r="B16" s="17">
+        <v>1</v>
+      </c>
       <c r="C16" s="6">
         <v>2</v>
       </c>
       <c r="D16" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E16" s="6">
         <v>1</v>
@@ -2084,13 +2202,15 @@
       <c r="G16" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="H16" s="17"/>
+      <c r="H16" s="17">
+        <v>2</v>
+      </c>
       <c r="I16" s="6">
         <v>2</v>
       </c>
       <c r="J16" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K16" s="23">
         <v>2</v>
@@ -2113,13 +2233,15 @@
       <c r="A17" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="17"/>
+      <c r="B17" s="17">
+        <v>1</v>
+      </c>
       <c r="C17" s="6">
         <v>2</v>
       </c>
       <c r="D17" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E17" s="6">
         <v>1</v>
@@ -2127,13 +2249,15 @@
       <c r="G17" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="H17" s="17"/>
+      <c r="H17" s="17">
+        <v>1</v>
+      </c>
       <c r="I17" s="6">
         <v>3</v>
       </c>
       <c r="J17" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K17" s="23">
         <v>1</v>
@@ -2168,13 +2292,15 @@
       <c r="G18" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="H18" s="17"/>
+      <c r="H18" s="17">
+        <v>2</v>
+      </c>
       <c r="I18" s="6">
         <v>1</v>
       </c>
       <c r="J18" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" s="23">
         <v>2</v>
@@ -2209,13 +2335,15 @@
       <c r="G19" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="17"/>
+      <c r="H19" s="17">
+        <v>2</v>
+      </c>
       <c r="I19" s="6">
         <v>3</v>
       </c>
       <c r="J19" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K19" s="23">
         <v>2</v>
@@ -2236,13 +2364,15 @@
       <c r="G20" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="H20" s="17"/>
+      <c r="H20" s="17">
+        <v>2</v>
+      </c>
       <c r="I20" s="6">
         <v>1</v>
       </c>
       <c r="J20" s="31">
         <f t="shared" ref="J20" si="6">(H20/K20)*I20</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="23">
         <v>2</v>

</xml_diff>